<commit_message>
Add shortcut compression method
</commit_message>
<xml_diff>
--- a/BinaryDefinitions.xlsx
+++ b/BinaryDefinitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keule\Documents\GitHub\F23P1-M013-Group11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC7CA62-8FFF-41A9-84EA-70153EA595DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A1F73F-9D47-4679-B9EE-5D3915FB9220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="73">
   <si>
     <t>Characters</t>
   </si>
@@ -231,12 +231,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>th</t>
-  </si>
-  <si>
-    <t>he</t>
-  </si>
-  <si>
     <t>in</t>
   </si>
   <si>
@@ -250,13 +244,19 @@
   </si>
   <si>
     <t>nd</t>
+  </si>
+  <si>
+    <t>::shortcut</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -277,6 +277,18 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -299,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -311,6 +323,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,8 +545,8 @@
   </sheetPr>
   <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -693,7 +707,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="1" t="str">
@@ -1425,8 +1439,8 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>66</v>
+      <c r="A75" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="B75" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1437,8 +1451,8 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>67</v>
+      <c r="A76" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="B76" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1450,7 +1464,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B77" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1462,7 +1476,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B78" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1474,7 +1488,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B79" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1486,7 +1500,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B80" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1498,7 +1512,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B81" s="1" t="str">
         <f t="shared" si="1"/>

</xml_diff>